<commit_message>
Update info capture from master_url file
</commit_message>
<xml_diff>
--- a/XX_Url/Afsupply.xlsx
+++ b/XX_Url/Afsupply.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OneDrive - Corona\03_Proy_ID\03_MACHINE_LEARNING\01_Projects\11_Web_Scrapping\Pricing\00_Sprint\00_Scrapping_code\XX_Url\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://orgcorona-my.sharepoint.com/personal/jmonsalvo_corona_com_co/Documents/03_Proy_ID/03_MACHINE_LEARNING/01_Projects/11_Web_Scrapping/Pricing/Scrapping_git/XX_Url/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45788529-374A-4F9D-A290-93C142411027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{45788529-374A-4F9D-A290-93C142411027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05E314AD-A775-42E3-8CCC-A3AD07AE4DD2}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>Linea</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Bowl Height</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>Link</t>
   </si>
   <si>
@@ -60,9 +57,6 @@
     <t>Fabricante</t>
   </si>
   <si>
-    <t>Homólogo Mansfield</t>
-  </si>
-  <si>
     <t>Gerber</t>
   </si>
   <si>
@@ -93,7 +87,43 @@
     <t>https://www.afsupply.com/gerber-gvp2859025-plumbing-viper-toilet-tank-1-6-gpf-12-rough-in-bone.html</t>
   </si>
   <si>
-    <t>Round</t>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Bowl</t>
+  </si>
+  <si>
+    <t>Maxwell</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>Round Front</t>
+  </si>
+  <si>
+    <t>Tank</t>
+  </si>
+  <si>
+    <t>Viper</t>
+  </si>
+  <si>
+    <t>Descripcion</t>
+  </si>
+  <si>
+    <t>Short Name</t>
+  </si>
+  <si>
+    <t>Gerber Maxwell Std RF Bowl</t>
+  </si>
+  <si>
+    <t>Gerber Viper 1,6 gpf Tank</t>
+  </si>
+  <si>
+    <t>Homologo Mansfield</t>
   </si>
 </sst>
 </file>
@@ -1004,10 +1034,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1015,97 +1045,129 @@
     <col min="1" max="1" width="21.5703125" customWidth="1"/>
     <col min="2" max="2" width="22.140625" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" customWidth="1"/>
-    <col min="9" max="9" width="87.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="214" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="97.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>4</v>
+      <c r="C2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="4">
+        <v>1.28</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="4" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="4">
-        <v>1.28</v>
-      </c>
-      <c r="I2" s="5" t="s">
+      <c r="D3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="G3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4" t="s">
+      <c r="K3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="H3" s="4">
-        <v>1.6</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>